<commit_message>
Updates on Results8-line and Results7-line
</commit_message>
<xml_diff>
--- a/Notes/Results7-lines.xlsx
+++ b/Notes/Results7-lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshitijbhatta/Desktop/Powergrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85B9B05-E1FB-2E40-8A51-8268B047CA5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010BAA04-72C1-CA46-9E43-9E172FE39197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="27640" windowHeight="15720" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="37">
   <si>
     <t>BEFORE FALIURE</t>
   </si>
@@ -137,10 +137,13 @@
     <t>INDEX</t>
   </si>
   <si>
-    <t>Max flow value</t>
-  </si>
-  <si>
     <t>Line 6-5 doesn't change with any faliure</t>
+  </si>
+  <si>
+    <t>After faliure peak flows</t>
+  </si>
+  <si>
+    <t>Max steady state flow value</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -232,6 +235,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205C97E-91D2-964B-9E2A-7A9AF5F69B57}">
-  <dimension ref="A2:S123"/>
+  <dimension ref="A2:S133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" workbookViewId="0">
+      <selection activeCell="N130" sqref="N130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3153,13 +3159,223 @@
     <row r="122" spans="1:13">
       <c r="B122" s="15"/>
       <c r="C122" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="123" spans="1:13">
       <c r="B123" s="11"/>
       <c r="C123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
+      <c r="E125" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" t="s">
+        <v>11</v>
+      </c>
+      <c r="G126" t="s">
+        <v>25</v>
+      </c>
+      <c r="H126" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
+      <c r="A127" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127">
+        <v>-0.21072859668057201</v>
+      </c>
+      <c r="D127">
+        <v>-0.17172798229996514</v>
+      </c>
+      <c r="E127">
+        <v>0.21850378415050509</v>
+      </c>
+      <c r="F127">
+        <v>0.21735098256099508</v>
+      </c>
+      <c r="G127">
+        <v>-0.18193897494577549</v>
+      </c>
+      <c r="H127">
+        <v>-0.14440009504045193</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" t="s">
+        <v>21</v>
+      </c>
+      <c r="B128">
+        <v>-0.19154410829660734</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D128">
+        <v>-0.1661907107952626</v>
+      </c>
+      <c r="E128">
+        <v>-5.0770978378311647E-2</v>
+      </c>
+      <c r="F128">
+        <v>0.19717317530171802</v>
+      </c>
+      <c r="G128">
+        <v>-0.1533113921391685</v>
+      </c>
+      <c r="H128">
+        <v>-0.10286545522743409</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>22</v>
+      </c>
+      <c r="B129">
+        <v>-0.17208826861394289</v>
+      </c>
+      <c r="C129">
+        <v>-0.16943811021055466</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E129">
+        <v>-4.808091681095443E-2</v>
+      </c>
+      <c r="F129">
+        <v>0.13472613233473418</v>
+      </c>
+      <c r="G129">
+        <v>-0.34734017213825741</v>
+      </c>
+      <c r="H129">
+        <v>-0.11997663201118036</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130">
+        <v>-0.16591309949330404</v>
+      </c>
+      <c r="C130">
+        <v>-7.8624007831761544E-2</v>
+      </c>
+      <c r="D130">
+        <v>-9.7209267636195862E-2</v>
+      </c>
+      <c r="E130" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F130">
+        <v>0.14021832113455973</v>
+      </c>
+      <c r="G130">
+        <v>-0.17386827121426249</v>
+      </c>
+      <c r="H130">
+        <v>-9.0121362104720229E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>24</v>
+      </c>
+      <c r="B131">
+        <v>-0.21721524443403384</v>
+      </c>
+      <c r="C131">
+        <v>-0.22923039995958008</v>
+      </c>
+      <c r="D131">
+        <v>0.15292218734029528</v>
+      </c>
+      <c r="E131">
+        <v>-5.3743232222505918E-2</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G131">
+        <v>-0.37192983108837596</v>
+      </c>
+      <c r="H131">
+        <v>-0.16040382230771827</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>29</v>
+      </c>
+      <c r="B132">
+        <v>-0.11213940654486677</v>
+      </c>
+      <c r="C132">
+        <v>0.10416578075885405</v>
+      </c>
+      <c r="D132">
+        <v>-0.39272386684044647</v>
+      </c>
+      <c r="E132">
+        <v>0.1371169877065529</v>
+      </c>
+      <c r="F132">
+        <v>0.38031601511440488</v>
+      </c>
+      <c r="G132" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H132">
+        <v>-0.17428290515186906</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133">
+        <v>-0.13894458643497695</v>
+      </c>
+      <c r="C133">
+        <v>-0.10071780035292241</v>
+      </c>
+      <c r="D133">
+        <v>-9.7209267636195862E-2</v>
+      </c>
+      <c r="E133">
+        <v>4.9004698911875755E-2</v>
+      </c>
+      <c r="F133">
+        <v>0.16500954553520242</v>
+      </c>
+      <c r="G133">
+        <v>-0.1533113921391685</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated values and added tables
</commit_message>
<xml_diff>
--- a/Notes/Results7-lines.xlsx
+++ b/Notes/Results7-lines.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshitijbhatta/Desktop/Powergrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010BAA04-72C1-CA46-9E43-9E172FE39197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD308ED-0314-CC4C-B4C3-4AAB669A220B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="38">
   <si>
     <t>BEFORE FALIURE</t>
   </si>
@@ -92,9 +114,6 @@
     <t>Steady State of thetaj-thetai</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Line 2-1</t>
   </si>
   <si>
@@ -143,7 +162,13 @@
     <t>After faliure peak flows</t>
   </si>
   <si>
-    <t>Max steady state flow value</t>
+    <t>10 s is time at faliure</t>
+  </si>
+  <si>
+    <t>Time for max flow after faliure</t>
+  </si>
+  <si>
+    <t>Differences insteady state after faliure and before faliure</t>
   </si>
 </sst>
 </file>
@@ -184,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,12 +219,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,10 +252,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -265,8 +286,8 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>394252</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>146838</xdr:rowOff>
     </xdr:to>
@@ -314,8 +335,8 @@
       <xdr:rowOff>279400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>292652</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -363,8 +384,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>317499</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>483151</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>149162</xdr:rowOff>
     </xdr:to>
@@ -412,8 +433,8 @@
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>457752</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>88899</xdr:rowOff>
     </xdr:to>
@@ -462,7 +483,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>682849</xdr:colOff>
+      <xdr:colOff>20240</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -510,8 +531,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>216452</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>42831</xdr:rowOff>
     </xdr:to>
@@ -559,8 +580,8 @@
       <xdr:rowOff>139699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>318052</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>93942</xdr:rowOff>
     </xdr:to>
@@ -609,7 +630,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>821004</xdr:colOff>
+      <xdr:colOff>158395</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>13240</xdr:rowOff>
     </xdr:to>
@@ -949,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205C97E-91D2-964B-9E2A-7A9AF5F69B57}">
-  <dimension ref="A2:S133"/>
+  <dimension ref="A2:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" workbookViewId="0">
-      <selection activeCell="N130" sqref="N130"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -965,9 +986,14 @@
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="31">
@@ -995,10 +1021,10 @@
         <v>11</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
       </c>
       <c r="K3" t="s">
         <v>4</v>
@@ -1252,10 +1278,10 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
         <v>25</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
       </c>
       <c r="K14" t="s">
         <v>17</v>
@@ -2418,7 +2444,7 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -2654,7 +2680,7 @@
     </row>
     <row r="92" spans="1:13">
       <c r="A92" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -2801,7 +2827,7 @@
         <v>0.1720877576469311</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:17">
       <c r="A97">
         <v>5</v>
       </c>
@@ -2837,7 +2863,7 @@
         <v>0.13961637660447176</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:17">
       <c r="A98">
         <v>6</v>
       </c>
@@ -2873,9 +2899,9 @@
         <v>0.12357349114787652</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:17">
       <c r="E101" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F101" t="s">
         <v>18</v>
@@ -2883,11 +2909,11 @@
       <c r="I101" s="7"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:17">
       <c r="I102" s="7"/>
       <c r="J102" s="6"/>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:17">
       <c r="B103" s="2">
         <v>-0.11038961</v>
       </c>
@@ -2912,27 +2938,32 @@
       <c r="I103" s="7"/>
       <c r="J103" s="6"/>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:17">
       <c r="I104" s="7"/>
       <c r="J104" s="6"/>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:17">
       <c r="I105" s="7"/>
       <c r="J105" s="6"/>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:17">
       <c r="I106" s="7"/>
       <c r="J106" s="6"/>
     </row>
-    <row r="109" spans="1:13">
+    <row r="108" spans="1:17">
+      <c r="M108" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17">
       <c r="E109" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F109" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:17">
       <c r="B110" t="s">
         <v>7</v>
       </c>
@@ -2949,15 +2980,36 @@
         <v>11</v>
       </c>
       <c r="G110" t="s">
+        <v>24</v>
+      </c>
+      <c r="H110" t="s">
         <v>25</v>
       </c>
-      <c r="H110" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="K110" t="s">
+        <v>7</v>
+      </c>
+      <c r="L110" t="s">
+        <v>8</v>
+      </c>
+      <c r="M110" t="s">
+        <v>9</v>
+      </c>
+      <c r="N110" t="s">
+        <v>10</v>
+      </c>
+      <c r="O110" t="s">
+        <v>11</v>
+      </c>
+      <c r="P110" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17">
       <c r="A111" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>12</v>
@@ -2980,10 +3032,35 @@
       <c r="H111" s="11">
         <v>-7.1428571428571355E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="J111" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K111" t="e" cm="1">
+        <f t="array" ref="K111:Q111">B111:H111-B103:H103</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L111">
+        <v>-8.2792207714285831E-2</v>
+      </c>
+      <c r="M111">
+        <v>-2.7597403000000006E-2</v>
+      </c>
+      <c r="N111">
+        <v>0.11038961085714291</v>
+      </c>
+      <c r="O111">
+        <v>2.759740271428579E-2</v>
+      </c>
+      <c r="P111">
+        <v>2.759740300000002E-2</v>
+      </c>
+      <c r="Q111">
+        <v>-4.2857135895690845E-10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17">
       <c r="A112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B112">
         <v>-0.15714285714285714</v>
@@ -3006,10 +3083,35 @@
       <c r="H112" s="11">
         <v>-7.1428571428571452E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="J112" t="s">
+        <v>20</v>
+      </c>
+      <c r="K112" cm="1">
+        <f t="array" ref="K112:Q112">B112:H112-B103:H103</f>
+        <v>-4.6753247142857141E-2</v>
+      </c>
+      <c r="L112" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M112">
+        <v>-3.1168831571428537E-2</v>
+      </c>
+      <c r="N112">
+        <v>-4.6753246285714284E-2</v>
+      </c>
+      <c r="O112">
+        <v>3.1168831285714294E-2</v>
+      </c>
+      <c r="P112">
+        <v>3.1168831571428621E-2</v>
+      </c>
+      <c r="Q112">
+        <v>-4.2857145610142311E-10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17">
       <c r="A113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B113">
         <v>-0.14285714285714288</v>
@@ -3033,13 +3135,35 @@
         <v>-7.1428571428571369E-2</v>
       </c>
       <c r="I113" s="4"/>
-      <c r="M113" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13">
+      <c r="J113" t="s">
+        <v>21</v>
+      </c>
+      <c r="K113" cm="1">
+        <f t="array" ref="K113:Q113">B113:H113-B103:H103</f>
+        <v>-3.2467532857142878E-2</v>
+      </c>
+      <c r="L113">
+        <v>-6.4935064857142843E-2</v>
+      </c>
+      <c r="M113" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N113">
+        <v>-3.2467531999999986E-2</v>
+      </c>
+      <c r="O113">
+        <v>-9.7402597285714279E-2</v>
+      </c>
+      <c r="P113">
+        <v>-9.7402597000000063E-2</v>
+      </c>
+      <c r="Q113">
+        <v>-4.2857137283469626E-10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B114">
         <v>-0.14285714285714285</v>
@@ -3062,10 +3186,35 @@
       <c r="H114" s="11">
         <v>-7.1428571428571452E-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="J114" t="s">
+        <v>22</v>
+      </c>
+      <c r="K114" cm="1">
+        <f t="array" ref="K114:Q114">B114:H114-B103:H103</f>
+        <v>-3.246753285714285E-2</v>
+      </c>
+      <c r="L114">
+        <v>2.4350649428571389E-2</v>
+      </c>
+      <c r="M114">
+        <v>8.1168827142856365E-3</v>
+      </c>
+      <c r="N114" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O114">
+        <v>-8.1168829999999637E-3</v>
+      </c>
+      <c r="P114">
+        <v>-8.1168827142857891E-3</v>
+      </c>
+      <c r="Q114">
+        <v>-4.2857145610142311E-10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B115">
         <v>-0.15476190476190468</v>
@@ -3088,10 +3237,35 @@
       <c r="H115" s="11">
         <v>-7.142857142857148E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="J115" t="s">
+        <v>23</v>
+      </c>
+      <c r="K115" cm="1">
+        <f t="array" ref="K115:Q115">B115:H115-B103:H103</f>
+        <v>-4.4372294761904685E-2</v>
+      </c>
+      <c r="L115">
+        <v>-8.8744588666666624E-2</v>
+      </c>
+      <c r="M115">
+        <v>0.13311688271428568</v>
+      </c>
+      <c r="N115">
+        <v>-4.4372293904761925E-2</v>
+      </c>
+      <c r="O115" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P115">
+        <v>-0.13311688271428559</v>
+      </c>
+      <c r="Q115">
+        <v>-4.2857148385699873E-10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17">
       <c r="A116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B116">
         <v>-5.9523809523809604E-2</v>
@@ -3114,10 +3288,35 @@
       <c r="H116" s="12">
         <v>-7.1428570999999996E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="J116" t="s">
+        <v>28</v>
+      </c>
+      <c r="K116" cm="1">
+        <f t="array" ref="K116:Q116">B116:H116-B103:H103</f>
+        <v>5.0865800476190395E-2</v>
+      </c>
+      <c r="L116">
+        <v>0.10173160180952379</v>
+      </c>
+      <c r="M116">
+        <v>-0.15259740299999996</v>
+      </c>
+      <c r="N116">
+        <v>5.0865801333333384E-2</v>
+      </c>
+      <c r="O116">
+        <v>0.15259740271428571</v>
+      </c>
+      <c r="P116" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B117">
         <v>-0.12077922077922076</v>
@@ -3126,7 +3325,7 @@
         <v>-8.4415584415584471E-2</v>
       </c>
       <c r="D117">
-        <v>-0.22748422165334192</v>
+        <v>-6.623376623376627E-2</v>
       </c>
       <c r="E117">
         <v>3.6363636363636292E-2</v>
@@ -3134,14 +3333,39 @@
       <c r="F117">
         <v>0.14480519480519474</v>
       </c>
-      <c r="G117" s="14">
-        <v>-0.28787383204295219</v>
+      <c r="G117">
+        <v>-0.12662337662337653</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="J117" t="s">
+        <v>29</v>
+      </c>
+      <c r="K117" cm="1">
+        <f t="array" ref="K117:Q117">B117:H117-B103:H103</f>
+        <v>-1.0389610779220765E-2</v>
+      </c>
+      <c r="L117">
+        <v>-6.4935064155844657E-3</v>
+      </c>
+      <c r="M117">
+        <v>3.1168830766233724E-2</v>
+      </c>
+      <c r="N117">
+        <v>3.8961043636362921E-3</v>
+      </c>
+      <c r="O117">
+        <v>1.1688311805194751E-2</v>
+      </c>
+      <c r="P117">
+        <v>2.5974026376623466E-2</v>
+      </c>
+      <c r="Q117" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17">
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
@@ -3151,29 +3375,34 @@
       <c r="H118" s="4"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:17">
       <c r="B121" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
       <c r="B122" s="15"/>
-      <c r="C122" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13">
+    </row>
+    <row r="123" spans="1:17">
       <c r="B123" s="11"/>
       <c r="C123" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17">
+      <c r="L124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="E125" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="125" spans="1:13">
-      <c r="E125" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13">
+      <c r="L125" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
       <c r="B126" t="s">
         <v>7</v>
       </c>
@@ -3190,17 +3419,39 @@
         <v>11</v>
       </c>
       <c r="G126" t="s">
+        <v>24</v>
+      </c>
+      <c r="H126" t="s">
         <v>25</v>
       </c>
-      <c r="H126" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13">
+      <c r="J126" s="7"/>
+      <c r="K126" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L126" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M126" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N126" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O126" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P126" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q126" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
       <c r="A127" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B127" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C127">
@@ -3221,10 +3472,34 @@
       <c r="H127">
         <v>-0.14440009504045193</v>
       </c>
-    </row>
-    <row r="128" spans="1:13">
+      <c r="J127" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K127" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L127" s="7">
+        <v>10.234</v>
+      </c>
+      <c r="M127" s="7">
+        <v>10.162000000000001</v>
+      </c>
+      <c r="N127" s="7">
+        <v>10.2538</v>
+      </c>
+      <c r="O127" s="7">
+        <v>10.340199999999999</v>
+      </c>
+      <c r="P127" s="7">
+        <v>10.7254</v>
+      </c>
+      <c r="Q127" s="7">
+        <v>10.7056</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17">
       <c r="A128" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B128">
         <v>-0.19154410829660734</v>
@@ -3247,10 +3522,34 @@
       <c r="H128">
         <v>-0.10286545522743409</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="J128" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K128" s="7">
+        <v>10.207000000000001</v>
+      </c>
+      <c r="L128" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M128" s="7">
+        <v>10.657</v>
+      </c>
+      <c r="N128" s="7">
+        <v>10.210599999999999</v>
+      </c>
+      <c r="O128" s="7">
+        <v>10.934200000000001</v>
+      </c>
+      <c r="P128" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q128" s="7">
+        <v>10.554399999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
       <c r="A129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B129">
         <v>-0.17208826861394289</v>
@@ -3273,10 +3572,34 @@
       <c r="H129">
         <v>-0.11997663201118036</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="J129" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K129" s="7">
+        <v>10.1548</v>
+      </c>
+      <c r="L129" s="7">
+        <v>10.410399999999999</v>
+      </c>
+      <c r="M129" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N129" s="7">
+        <v>10.621</v>
+      </c>
+      <c r="O129" s="7">
+        <v>10</v>
+      </c>
+      <c r="P129" s="7">
+        <v>10.446400000000001</v>
+      </c>
+      <c r="Q129" s="7">
+        <v>10.415800000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B130">
         <v>-0.16591309949330404</v>
@@ -3299,10 +3622,34 @@
       <c r="H130">
         <v>-9.0121362104720229E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="J130" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K130" s="7">
+        <v>10.246600000000001</v>
+      </c>
+      <c r="L130" s="7">
+        <v>10</v>
+      </c>
+      <c r="M130" s="7">
+        <v>10</v>
+      </c>
+      <c r="N130" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O130" s="7">
+        <v>10.331200000000001</v>
+      </c>
+      <c r="P130" s="7">
+        <v>10.266400000000001</v>
+      </c>
+      <c r="Q130" s="7">
+        <v>11.3248</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17">
       <c r="A131" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B131">
         <v>-0.21721524443403384</v>
@@ -3325,10 +3672,34 @@
       <c r="H131">
         <v>-0.16040382230771827</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="J131" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K131" s="7">
+        <v>10.3474</v>
+      </c>
+      <c r="L131" s="7">
+        <v>10.426600000000001</v>
+      </c>
+      <c r="M131" s="7">
+        <v>10.441000000000001</v>
+      </c>
+      <c r="N131" s="7">
+        <v>10.1548</v>
+      </c>
+      <c r="O131" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P131" s="7">
+        <v>10.3222</v>
+      </c>
+      <c r="Q131" s="7">
+        <v>10.784800000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B132">
         <v>-0.11213940654486677</v>
@@ -3351,10 +3722,34 @@
       <c r="H132">
         <v>-0.17428290515186906</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="J132" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K132" s="7">
+        <v>10.7056</v>
+      </c>
+      <c r="L132" s="7">
+        <v>11.250999999999999</v>
+      </c>
+      <c r="M132" s="7">
+        <v>10.4338</v>
+      </c>
+      <c r="N132" s="7">
+        <v>10.2844</v>
+      </c>
+      <c r="O132" s="7">
+        <v>10.315</v>
+      </c>
+      <c r="P132" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q132" s="7">
+        <v>10.387</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17">
       <c r="A133" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B133">
         <v>-0.13894458643497695</v>
@@ -3377,6 +3772,40 @@
       <c r="H133" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="J133" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K133" s="7">
+        <v>10.230399999999999</v>
+      </c>
+      <c r="L133" s="7">
+        <v>10.5022</v>
+      </c>
+      <c r="M133" s="7">
+        <v>10</v>
+      </c>
+      <c r="N133" s="7">
+        <v>11.097999999999999</v>
+      </c>
+      <c r="O133" s="7">
+        <v>10.703799999999999</v>
+      </c>
+      <c r="P133" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q133" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17">
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+      <c r="L134" s="7"/>
+      <c r="M134" s="7"/>
+      <c r="N134" s="7"/>
+      <c r="O134" s="7"/>
+      <c r="P134" s="7"/>
+      <c r="Q134" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tables and added a few
</commit_message>
<xml_diff>
--- a/Notes/Results7-lines.xlsx
+++ b/Notes/Results7-lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshitijbhatta/Desktop/Powergrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD308ED-0314-CC4C-B4C3-4AAB669A220B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1634ED38-3ABF-0F45-8B47-B64A516635BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{F15564B4-478A-5749-9F90-458B4D70CD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="41">
   <si>
     <t>BEFORE FALIURE</t>
   </si>
@@ -170,6 +170,15 @@
   <si>
     <t>Differences insteady state after faliure and before faliure</t>
   </si>
+  <si>
+    <t>Zeta</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
 </sst>
 </file>
 
@@ -280,14 +289,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>394252</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>119932</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>146838</xdr:rowOff>
     </xdr:to>
@@ -329,14 +338,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>279400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>292652</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>18332</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -378,14 +387,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>483151</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>208831</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>149162</xdr:rowOff>
     </xdr:to>
@@ -427,14 +436,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>457752</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>183432</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>88899</xdr:rowOff>
     </xdr:to>
@@ -476,14 +485,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>247198</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>20240</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>568880</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -525,14 +534,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>216452</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>765092</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>42831</xdr:rowOff>
     </xdr:to>
@@ -574,14 +583,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>139699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>318052</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>43732</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>93942</xdr:rowOff>
     </xdr:to>
@@ -623,14 +632,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>573859</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>158395</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>707035</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>13240</xdr:rowOff>
     </xdr:to>
@@ -970,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205C97E-91D2-964B-9E2A-7A9AF5F69B57}">
-  <dimension ref="A2:S134"/>
+  <dimension ref="A2:V134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+    <sheetView tabSelected="1" topLeftCell="K75" zoomScale="125" workbookViewId="0">
+      <selection activeCell="P111" sqref="P111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -996,12 +1005,12 @@
     <col min="17" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="31">
+    <row r="2" spans="1:22" ht="31">
       <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1035,8 +1044,17 @@
       <c r="M3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1061,22 +1079,31 @@
       <c r="H4" s="10">
         <v>1.11022E-16</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="2">
+      <c r="P4">
         <v>0</v>
       </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1110,8 +1137,17 @@
       <c r="M5" s="2">
         <v>0.31287970900000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="N5" s="2">
+        <v>4.4771776999999999E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>10.050974800000001</v>
+      </c>
+      <c r="P5">
+        <v>-9.0319956618477555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1145,8 +1181,17 @@
       <c r="M6" s="2">
         <v>0.20477932900000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="N6" s="2">
+        <v>2.9319867999999999E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>15.347954700000001</v>
+      </c>
+      <c r="P6">
+        <v>29.356235817302444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1180,8 +1225,17 @@
       <c r="M7" s="2">
         <v>0.153330993</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="N7" s="2">
+        <v>2.1957752000000001E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>20.4939015</v>
+      </c>
+      <c r="P7">
+        <v>12.990381056766557</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1215,8 +1269,17 @@
       <c r="M8" s="2">
         <v>0.13797441599999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="N8" s="2">
+        <v>1.9759520999999999E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>22.773831699999999</v>
+      </c>
+      <c r="P8">
+        <v>5.5893788602955725</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1250,18 +1313,27 @@
       <c r="M9" s="2">
         <v>0.12007192899999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="31">
+      <c r="N9" s="2">
+        <v>1.7196494E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>26.168125199999999</v>
+      </c>
+      <c r="P9">
+        <v>61.69800091542173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="31">
       <c r="I12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:22">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -1292,8 +1364,17 @@
       <c r="M14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="N14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1318,17 +1399,26 @@
       <c r="H15">
         <v>1.6653345369377348E-16</v>
       </c>
-      <c r="K15">
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15">
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="P15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1362,8 +1452,17 @@
       <c r="M16">
         <v>0.34733859513408888</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>4.9691126197618889E-2</v>
+      </c>
+      <c r="O16">
+        <v>9.0559428701691047</v>
+      </c>
+      <c r="P16">
+        <v>6.5328148243818998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1397,8 +1496,17 @@
       <c r="M17">
         <v>0.23592979150847712</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>3.3775172068447143E-2</v>
+      </c>
+      <c r="O17">
+        <v>13.3233962239497</v>
+      </c>
+      <c r="P17">
+        <v>-41.9187270437981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1432,8 +1540,17 @@
       <c r="M18">
         <v>0.18781399808919713</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18">
+        <v>2.6892643710023856E-2</v>
+      </c>
+      <c r="O18">
+        <v>16.733200530681511</v>
+      </c>
+      <c r="P18">
+        <v>8.3262945336626329E-15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1467,8 +1584,17 @@
       <c r="M19">
         <v>0.14372506939190241</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>2.0582738400646741E-2</v>
+      </c>
+      <c r="O19">
+        <v>21.862980097238193</v>
+      </c>
+      <c r="P19">
+        <v>-2.7059805007309659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1502,25 +1628,34 @@
       <c r="M20">
         <v>0.1220752268845658</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>1.7483315565857634E-2</v>
+      </c>
+      <c r="O20">
+        <v>25.738825013190539</v>
+      </c>
+      <c r="P20">
+        <v>-56.060862667529051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:16">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:16">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:16">
       <c r="B24" s="7"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1546,17 +1681,26 @@
         <v>2.2204460492503131E-16</v>
       </c>
       <c r="J27" s="4"/>
-      <c r="K27">
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27">
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="P27">
         <v>0</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1591,8 +1735,17 @@
       <c r="M28">
         <v>0.31831018080002127</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28">
+        <v>4.554725611516882E-2</v>
+      </c>
+      <c r="O28">
+        <v>9.879848719364114</v>
+      </c>
+      <c r="P28">
+        <v>-5.6112252389563171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1627,8 +1780,17 @@
       <c r="M29">
         <v>0.2259771718776363</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29">
+        <v>3.2351901748514031E-2</v>
+      </c>
+      <c r="O29">
+        <v>13.90953779156643</v>
+      </c>
+      <c r="P29">
+        <v>-1.8587401723009245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1663,8 +1825,17 @@
       <c r="M30">
         <v>0.18781399808919713</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30">
+        <v>2.6892643710023856E-2</v>
+      </c>
+      <c r="O30">
+        <v>16.733200530681511</v>
+      </c>
+      <c r="P30">
+        <v>-44.907311951024951</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1699,8 +1870,17 @@
       <c r="M31">
         <v>0.13961637660447176</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31">
+        <v>1.9994574881278825E-2</v>
+      </c>
+      <c r="O31">
+        <v>22.506104914555635</v>
+      </c>
+      <c r="P31">
+        <v>-3.0075047750377304</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32">
         <v>6</v>
       </c>
@@ -1735,29 +1915,38 @@
       <c r="M32">
         <v>0.12802197218149247</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>1.8334714235392447E-2</v>
+      </c>
+      <c r="O32">
+        <v>24.543605873678779</v>
+      </c>
+      <c r="P32">
+        <v>53.752650954636941</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="C33" s="7"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:16">
       <c r="C34" s="7"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:16">
       <c r="C35" s="7"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:16">
       <c r="C36" s="7"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1782,17 +1971,26 @@
       <c r="H39">
         <v>-2.2204460492503131E-16</v>
       </c>
-      <c r="K39">
+      <c r="K39" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" t="s">
+        <v>12</v>
+      </c>
+      <c r="N39" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39">
         <v>0</v>
       </c>
-      <c r="L39">
+      <c r="P39">
         <v>0</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1826,8 +2024,17 @@
       <c r="M40">
         <v>0.46687498487418394</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40">
+        <v>6.6725874395287169E-2</v>
+      </c>
+      <c r="O40">
+        <v>6.7440105368148364</v>
+      </c>
+      <c r="P40">
+        <v>-14.750069403610786</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1861,8 +2068,17 @@
       <c r="M41">
         <v>0.21978797946973322</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41">
+        <v>3.1466718994747518E-2</v>
+      </c>
+      <c r="O41">
+        <v>14.300823675805374</v>
+      </c>
+      <c r="P41">
+        <v>18.827355355898227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1896,8 +2112,17 @@
       <c r="M42">
         <v>0.15333099316873319</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42">
+        <v>2.1957751641341998E-2</v>
+      </c>
+      <c r="O42">
+        <v>20.493901531919196</v>
+      </c>
+      <c r="P42">
+        <v>16.431676725155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1931,8 +2156,17 @@
       <c r="M43">
         <v>0.15333099316873319</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43">
+        <v>2.1957751641341998E-2</v>
+      </c>
+      <c r="O43">
+        <v>20.493901531919196</v>
+      </c>
+      <c r="P43">
+        <v>42.42640687119286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>6</v>
       </c>
@@ -1966,25 +2200,34 @@
       <c r="M44">
         <v>0.12935900160587505</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44">
+        <v>1.8526132019508069E-2</v>
+      </c>
+      <c r="O44">
+        <v>24.290013669672046</v>
+      </c>
+      <c r="P44">
+        <v>48.041296224096556</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:16">
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:16">
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:16">
       <c r="D48" s="7"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:16">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2009,17 +2252,26 @@
       <c r="H51">
         <v>-5.5511151231257827E-17</v>
       </c>
-      <c r="K51">
+      <c r="K51" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51">
         <v>0</v>
       </c>
-      <c r="L51">
+      <c r="P51">
         <v>0</v>
       </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>2</v>
       </c>
@@ -2053,8 +2305,17 @@
       <c r="M52">
         <v>0.32791122545301948</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52">
+        <v>4.6918097181573221E-2</v>
+      </c>
+      <c r="O52">
+        <v>9.5911818047202182</v>
+      </c>
+      <c r="P52">
+        <v>-1.8394037549092108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2088,8 +2349,17 @@
       <c r="M53">
         <v>0.26570527116581932</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53">
+        <v>3.8031941462783228E-2</v>
+      </c>
+      <c r="O53">
+        <v>11.832159566199238</v>
+      </c>
+      <c r="P53">
+        <v>-22.500000000000028</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54">
         <v>4</v>
       </c>
@@ -2123,8 +2393,17 @@
       <c r="M54">
         <v>0.16699692483636883</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54">
+        <v>2.3913706817439307E-2</v>
+      </c>
+      <c r="O54">
+        <v>18.817659823103337</v>
+      </c>
+      <c r="P54">
+        <v>-19.308270747018128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2158,8 +2437,17 @@
       <c r="M55">
         <v>0.15333099316873317</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55">
+        <v>2.1957751641341994E-2</v>
+      </c>
+      <c r="O55">
+        <v>20.493901531919199</v>
+      </c>
+      <c r="P55">
+        <v>12.990381056766559</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56">
         <v>6</v>
       </c>
@@ -2193,28 +2481,37 @@
       <c r="M56">
         <v>0.12103635099751386</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56">
+        <v>1.7334575200901873E-2</v>
+      </c>
+      <c r="O56">
+        <v>25.959678549064627</v>
+      </c>
+      <c r="P56">
+        <v>-62.440429807827798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:16">
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:16">
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:16">
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:16">
       <c r="E61" s="7"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:16">
       <c r="A64">
         <v>1</v>
       </c>
@@ -2239,17 +2536,26 @@
       <c r="H64">
         <v>-1.1102230246251565E-16</v>
       </c>
-      <c r="K64">
+      <c r="K64" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" t="s">
+        <v>12</v>
+      </c>
+      <c r="M64" t="s">
+        <v>12</v>
+      </c>
+      <c r="N64" t="s">
+        <v>12</v>
+      </c>
+      <c r="O64">
         <v>0</v>
       </c>
-      <c r="L64">
+      <c r="P64">
         <v>0</v>
       </c>
-      <c r="M64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2283,8 +2589,17 @@
       <c r="M65">
         <v>0.40164721451273289</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65">
+        <v>5.7436749205221641E-2</v>
+      </c>
+      <c r="O65">
+        <v>7.8347052405794928</v>
+      </c>
+      <c r="P65">
+        <v>17.890714076721789</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66">
         <v>3</v>
       </c>
@@ -2318,8 +2633,17 @@
       <c r="M66">
         <v>0.26570527116581943</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66">
+        <v>3.8031941462783242E-2</v>
+      </c>
+      <c r="O66">
+        <v>11.832159566199234</v>
+      </c>
+      <c r="P66">
+        <v>-35.355339059327385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67">
         <v>4</v>
       </c>
@@ -2353,8 +2677,17 @@
       <c r="M67">
         <v>0.15333099316873322</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67">
+        <v>2.1957751641342001E-2</v>
+      </c>
+      <c r="O67">
+        <v>20.493901531919192</v>
+      </c>
+      <c r="P67">
+        <v>-12.990381056766577</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68">
         <v>5</v>
       </c>
@@ -2388,8 +2721,17 @@
       <c r="M68">
         <v>0.15333099316873319</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68">
+        <v>2.1957751641341998E-2</v>
+      </c>
+      <c r="O68">
+        <v>20.493901531919196</v>
+      </c>
+      <c r="P68">
+        <v>-3.5355339059327298</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69">
         <v>6</v>
       </c>
@@ -2423,31 +2765,40 @@
       <c r="M69">
         <v>0.12433642255594364</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69">
+        <v>1.7807056727822807E-2</v>
+      </c>
+      <c r="O69">
+        <v>25.270880352556702</v>
+      </c>
+      <c r="P69">
+        <v>56.556806396975674</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:16">
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:16">
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:16">
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:16">
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:16">
       <c r="F75" s="7"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:16">
       <c r="A77" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:16">
       <c r="A78">
         <v>1</v>
       </c>
@@ -2472,17 +2823,26 @@
       <c r="H78">
         <v>-1.1102230246251565E-16</v>
       </c>
-      <c r="K78">
+      <c r="K78" t="s">
+        <v>12</v>
+      </c>
+      <c r="L78" t="s">
+        <v>12</v>
+      </c>
+      <c r="M78" t="s">
+        <v>12</v>
+      </c>
+      <c r="N78" t="s">
+        <v>12</v>
+      </c>
+      <c r="O78">
         <v>0</v>
       </c>
-      <c r="L78">
+      <c r="P78">
         <v>0</v>
       </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79">
         <v>2</v>
       </c>
@@ -2516,8 +2876,17 @@
       <c r="M79">
         <v>0.41383104508832469</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79">
+        <v>5.917306214245379E-2</v>
+      </c>
+      <c r="O79">
+        <v>7.6048117793306984</v>
+      </c>
+      <c r="P79">
+        <v>26.911851442139472</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80">
         <v>3</v>
       </c>
@@ -2551,8 +2920,17 @@
       <c r="M80">
         <v>0.24916949035667849</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80">
+        <v>3.5668189892068311E-2</v>
+      </c>
+      <c r="O80">
+        <v>12.616283623074139</v>
+      </c>
+      <c r="P80">
+        <v>-24.516927016353776</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2586,8 +2964,17 @@
       <c r="M81">
         <v>0.17290667584602629</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81">
+        <v>2.4759464287493201E-2</v>
+      </c>
+      <c r="O81">
+        <v>18.174868194838506</v>
+      </c>
+      <c r="P81">
+        <v>12.570911559177622</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82">
         <v>5</v>
       </c>
@@ -2621,8 +3008,17 @@
       <c r="M82">
         <v>0.1381027229702412</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82">
+        <v>1.9777888570779483E-2</v>
+      </c>
+      <c r="O82">
+        <v>22.752681530668806</v>
+      </c>
+      <c r="P82">
+        <v>9.1789657183506357</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83">
         <v>6</v>
       </c>
@@ -2656,34 +3052,43 @@
       <c r="M83">
         <v>0.12670355941175132</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83">
+        <v>1.8145959757744776E-2</v>
+      </c>
+      <c r="O83">
+        <v>24.798908738235134</v>
+      </c>
+      <c r="P83">
+        <v>58.15832969183068</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:16">
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:16">
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:16">
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:16">
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:16">
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:16">
       <c r="G90" s="7"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:16">
       <c r="A92" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:16">
       <c r="A93">
         <v>1</v>
       </c>
@@ -2709,17 +3114,26 @@
         <v>12</v>
       </c>
       <c r="I93" s="5"/>
-      <c r="K93">
+      <c r="K93" t="s">
+        <v>12</v>
+      </c>
+      <c r="L93" t="s">
+        <v>12</v>
+      </c>
+      <c r="M93" t="s">
+        <v>12</v>
+      </c>
+      <c r="N93" t="s">
+        <v>12</v>
+      </c>
+      <c r="O93">
         <v>0</v>
       </c>
-      <c r="L93">
-        <v>0</v>
-      </c>
-      <c r="M93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="P93">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94">
         <v>2</v>
       </c>
@@ -2745,17 +3159,26 @@
         <v>12</v>
       </c>
       <c r="I94" s="6"/>
-      <c r="K94">
-        <v>-726207490940923.62</v>
-      </c>
-      <c r="L94">
+      <c r="K94" t="s">
+        <v>12</v>
+      </c>
+      <c r="L94" t="s">
+        <v>12</v>
+      </c>
+      <c r="M94" t="s">
+        <v>12</v>
+      </c>
+      <c r="N94" t="s">
+        <v>12</v>
+      </c>
+      <c r="O94">
         <v>0</v>
       </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="P94">
+        <v>-4.4721359549995618</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95">
         <v>3</v>
       </c>
@@ -2790,8 +3213,17 @@
       <c r="M95">
         <v>0.22597717187763627</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="N95">
+        <v>3.2351901748514031E-2</v>
+      </c>
+      <c r="O95">
+        <v>13.909537791566432</v>
+      </c>
+      <c r="P95">
+        <v>17.392527130926076</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
       <c r="A96">
         <v>4</v>
       </c>
@@ -2826,6 +3258,15 @@
       <c r="M96">
         <v>0.1720877576469311</v>
       </c>
+      <c r="N96">
+        <v>2.4642270234029123E-2</v>
+      </c>
+      <c r="O96">
+        <v>18.261304487221466</v>
+      </c>
+      <c r="P96">
+        <v>-14.933939835578476</v>
+      </c>
     </row>
     <row r="97" spans="1:17">
       <c r="A97">
@@ -2862,6 +3303,15 @@
       <c r="M97">
         <v>0.13961637660447176</v>
       </c>
+      <c r="N97">
+        <v>1.9994574881278829E-2</v>
+      </c>
+      <c r="O97">
+        <v>22.506104914555632</v>
+      </c>
+      <c r="P97">
+        <v>17.392527130926062</v>
+      </c>
     </row>
     <row r="98" spans="1:17">
       <c r="A98">
@@ -2897,6 +3347,15 @@
       </c>
       <c r="M98">
         <v>0.12357349114787652</v>
+      </c>
+      <c r="N98">
+        <v>1.7697826509705295E-2</v>
+      </c>
+      <c r="O98">
+        <v>25.426851130743366</v>
+      </c>
+      <c r="P98">
+        <v>63.261184315402446</v>
       </c>
     </row>
     <row r="101" spans="1:17">

</xml_diff>